<commit_message>
Using mass compartments for diffuse layer volumes
This is exploding/not converging when running the full organic problem, so still WIP
</commit_message>
<xml_diff>
--- a/scrap/manual speciation calculations - abbrev organic only.xlsx
+++ b/scrap/manual speciation calculations - abbrev organic only.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kellyc\Documents\BLM Development\engine\BLMEngineInR\scrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C2083A-455D-40A0-A34B-659F237E5DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E188F3-B2F1-4CDC-871A-756F6142603D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{071414EE-D145-41C9-AE04-224A7CE52B17}"/>
   </bookViews>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="120">
   <si>
     <t>H</t>
   </si>
@@ -387,16 +387,67 @@
     <t>NSpec</t>
   </si>
   <si>
-    <t>double DL</t>
-  </si>
-  <si>
-    <t>double Cu</t>
-  </si>
-  <si>
     <t>WHAMSpecCharge[iFA]</t>
   </si>
   <si>
     <t>CalcTotMoles[4]</t>
+  </si>
+  <si>
+    <t>Jacobian[4, 0]</t>
+  </si>
+  <si>
+    <t>Jacobian[4, 1]</t>
+  </si>
+  <si>
+    <t>Jacobian[4, 2]</t>
+  </si>
+  <si>
+    <t>Jacobian[4, 4]</t>
+  </si>
+  <si>
+    <t>Jacobian[0, 4]</t>
+  </si>
+  <si>
+    <t>Jacobian[1, 4]</t>
+  </si>
+  <si>
+    <t>Jacobian[2, 4]</t>
+  </si>
+  <si>
+    <t>d R.DL / d DL</t>
+  </si>
+  <si>
+    <t>d R.DL / d Cu</t>
+  </si>
+  <si>
+    <t>d R.DL / d Na</t>
+  </si>
+  <si>
+    <t>d R.DL / d Cl</t>
+  </si>
+  <si>
+    <t>d R.Cu / d DL</t>
+  </si>
+  <si>
+    <t>d R.Na / d DL</t>
+  </si>
+  <si>
+    <t>d R.Cl / d DL</t>
+  </si>
+  <si>
+    <t>Resid[4]</t>
+  </si>
+  <si>
+    <t>SpecCtoM[4]</t>
+  </si>
+  <si>
+    <t>SpecCtoM[0]</t>
+  </si>
+  <si>
+    <t>radius</t>
+  </si>
+  <si>
+    <t>MolWt</t>
   </si>
 </sst>
 </file>
@@ -487,7 +538,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -516,30 +567,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -564,23 +595,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -604,23 +624,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -939,7 +952,7 @@
   <dimension ref="A1:X440"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3818,20 +3831,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBC2854-FB48-4B0B-92C4-9627756EEF9C}">
-  <dimension ref="A1:X28"/>
+  <dimension ref="A2:X48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.7109375" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -3846,16 +3858,8 @@
     <col min="23" max="24" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="E1" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="F1" t="s">
-        <v>100</v>
-      </c>
-    </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="16" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -3880,26 +3884,26 @@
       <c r="N2" s="18"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="22">
-        <v>0</v>
-      </c>
-      <c r="B3" s="23" t="str" cm="1">
+      <c r="A3" s="19">
+        <v>0</v>
+      </c>
+      <c r="B3" s="20" t="str" cm="1">
         <f t="array" ref="B3:B25">TRANSPOSE(SpecName)</f>
         <v>Cu</v>
       </c>
-      <c r="C3" s="23" cm="1">
-        <f t="array" aca="1" ref="C3:C25" ca="1">TRANSPOSE(SpecKTempAdj)</f>
-        <v>1</v>
-      </c>
-      <c r="D3" s="24">
-        <v>9.9999887798122905E-19</v>
-      </c>
-      <c r="E3" s="24">
-        <v>2.7167020134752897E-7</v>
-      </c>
-      <c r="F3" s="25">
-        <f>D3*2</f>
-        <v>1.9999977559624581E-18</v>
+      <c r="C3" s="20">
+        <v>1</v>
+      </c>
+      <c r="D3" s="21">
+        <v>6.4178960059668199E-7</v>
+      </c>
+      <c r="E3" s="21">
+        <f>D3</f>
+        <v>6.4178960059668199E-7</v>
+      </c>
+      <c r="F3" s="21">
+        <f>E3</f>
+        <v>6.4178960059668199E-7</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -3921,152 +3925,157 @@
       <c r="X3" s="2"/>
     </row>
     <row r="4" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26">
-        <v>1</v>
-      </c>
-      <c r="B4" s="27" t="str">
+      <c r="A4" s="22">
+        <v>1</v>
+      </c>
+      <c r="B4" s="23" t="str">
         <v>Na</v>
       </c>
-      <c r="C4" s="27">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="D4" s="28">
-        <v>9.9999900000100001E-10</v>
-      </c>
-      <c r="E4" s="28">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="F4" s="29">
-        <v>5.0000000000000001E-4</v>
+      <c r="C4" s="23">
+        <v>1</v>
+      </c>
+      <c r="D4" s="18">
+        <v>9.9999999999999005E-4</v>
+      </c>
+      <c r="E4" s="18">
+        <f t="shared" ref="E4:F9" si="0">D4</f>
+        <v>9.9999999999999005E-4</v>
+      </c>
+      <c r="F4" s="18">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999005E-4</v>
       </c>
     </row>
     <row r="5" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30">
+      <c r="A5" s="24">
         <v>2</v>
       </c>
-      <c r="B5" s="31" t="str">
+      <c r="B5" t="str">
         <v>Cl</v>
       </c>
-      <c r="C5" s="31">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="D5" s="28">
-        <v>2.9999970000029898E-10</v>
-      </c>
-      <c r="E5" s="28">
-        <v>2.9999999969297257E-4</v>
-      </c>
-      <c r="F5" s="29">
-        <v>2.9999999969297257E-4</v>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="18">
+        <v>2.9999956941106399E-4</v>
+      </c>
+      <c r="E5" s="18">
+        <f t="shared" si="0"/>
+        <v>2.9999956941106399E-4</v>
+      </c>
+      <c r="F5" s="18">
+        <f t="shared" si="0"/>
+        <v>2.9999956941106399E-4</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="30">
+      <c r="A6" s="24">
         <v>3</v>
       </c>
-      <c r="B6" s="31" t="str">
+      <c r="B6" t="str">
         <v>H</v>
       </c>
-      <c r="C6" s="31">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="D6" s="28">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="18">
         <v>2.6915348039269101E-8</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="18">
+        <f t="shared" si="0"/>
         <v>2.6915348039269101E-8</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="18">
+        <f t="shared" si="0"/>
         <v>2.6915348039269101E-8</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="26">
+      <c r="A7" s="22">
         <v>4</v>
       </c>
-      <c r="B7" s="31" t="str">
+      <c r="B7" t="str">
         <v>DonnanFA</v>
       </c>
-      <c r="C7" s="31">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="D7" s="28">
-        <v>1000000</v>
-      </c>
-      <c r="E7" s="28">
-        <v>2</v>
-      </c>
-      <c r="F7" s="29">
-        <v>1</v>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="18">
+        <v>889127.37023895502</v>
+      </c>
+      <c r="E7" s="18">
+        <f t="shared" si="0"/>
+        <v>889127.37023895502</v>
+      </c>
+      <c r="F7" s="18">
+        <f t="shared" si="0"/>
+        <v>889127.37023895502</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="30">
+      <c r="A8" s="24">
         <v>5</v>
       </c>
-      <c r="B8" s="31" t="str">
+      <c r="B8" t="str">
         <v>DOC-FA_1H</v>
       </c>
-      <c r="C8" s="31">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="D8" s="28">
-        <v>7.4293692689164605E-13</v>
-      </c>
-      <c r="E8" s="28">
-        <v>7.4293692479644037E-14</v>
-      </c>
-      <c r="F8" s="29">
-        <v>7.4293692479644037E-14</v>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="18">
+        <v>7.4293068803167404E-14</v>
+      </c>
+      <c r="E8" s="18">
+        <f t="shared" si="0"/>
+        <v>7.4293068803167404E-14</v>
+      </c>
+      <c r="F8" s="18">
+        <f t="shared" si="0"/>
+        <v>7.4293068803167404E-14</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="32">
+      <c r="A9" s="25">
         <v>6</v>
       </c>
-      <c r="B9" s="33" t="str">
+      <c r="B9" s="26" t="str">
         <v>DOC-FA_8H</v>
       </c>
-      <c r="C9" s="33">
-        <f ca="1"/>
-        <v>1</v>
-      </c>
-      <c r="D9" s="34">
-        <v>3.5474475294058302E-7</v>
-      </c>
-      <c r="E9" s="34">
-        <v>3.5474065863761704E-8</v>
-      </c>
-      <c r="F9" s="35">
-        <v>3.5474065863761704E-8</v>
+      <c r="C9" s="26">
+        <v>1</v>
+      </c>
+      <c r="D9" s="27">
+        <v>3.4295805959358799E-8</v>
+      </c>
+      <c r="E9" s="27">
+        <f t="shared" si="0"/>
+        <v>3.4295805959358799E-8</v>
+      </c>
+      <c r="F9" s="27">
+        <f t="shared" si="0"/>
+        <v>3.4295805959358799E-8</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>7</v>
       </c>
-      <c r="B10" s="20" t="str">
+      <c r="B10" t="str">
         <v>OH</v>
       </c>
-      <c r="C10" s="20">
-        <f ca="1"/>
+      <c r="C10">
         <v>2.1995725798065139E-14</v>
       </c>
       <c r="D10" s="18">
-        <f ca="1">$C10/D6</f>
+        <f>$C10/D6</f>
         <v>8.1721870235427371E-7</v>
       </c>
       <c r="E10" s="18">
-        <f ca="1">$C10/E6</f>
+        <f>$C10/E6</f>
         <v>8.1721870235427371E-7</v>
       </c>
       <c r="F10" s="18">
-        <f ca="1">$C10/F6</f>
+        <f>$C10/F6</f>
         <v>8.1721870235427371E-7</v>
       </c>
       <c r="G10" s="17"/>
@@ -4079,379 +4088,653 @@
       <c r="N10" s="18"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="21">
+      <c r="A11">
         <v>8</v>
       </c>
-      <c r="B11" s="20" t="str">
+      <c r="B11" t="str">
         <v>CuOH</v>
       </c>
-      <c r="C11" s="20">
-        <f ca="1"/>
+      <c r="C11">
         <v>1.4954498711240171E-8</v>
       </c>
       <c r="D11" s="18">
-        <f ca="1">$C11*D3/D6</f>
-        <v>5.5561168706395832E-19</v>
+        <f>$C11*D3/D6</f>
+        <v>3.5658620282403948E-7</v>
       </c>
       <c r="E11" s="18">
-        <f ca="1">$C11*E3/E6</f>
-        <v>1.5094330825693102E-7</v>
+        <f>$C11*E3/E6</f>
+        <v>3.5658620282403948E-7</v>
       </c>
       <c r="F11" s="18">
-        <f ca="1">$C11*F3/F6</f>
-        <v>1.1112233741279166E-18</v>
+        <f>$C11*F3/F6</f>
+        <v>3.5658620282403948E-7</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="21">
+      <c r="A12">
         <v>9</v>
       </c>
-      <c r="B12" s="20" t="str">
+      <c r="B12" t="str">
         <v>CuCl</v>
       </c>
-      <c r="C12" s="20">
-        <f ca="1"/>
+      <c r="C12">
         <v>2.2363202312453416</v>
       </c>
       <c r="D12" s="18">
-        <f ca="1">$C12*D3*D5</f>
-        <v>6.7089464572097129E-28</v>
+        <f>$C12*D3*D5</f>
+        <v>4.3057350240366027E-10</v>
       </c>
       <c r="E12" s="18">
-        <f ca="1">$C12*E3*E5</f>
-        <v>1.8226247006346043E-10</v>
+        <f>$C12*E3*E5</f>
+        <v>4.3057350240366027E-10</v>
       </c>
       <c r="F12" s="18">
-        <f ca="1">$C12*F3*F5</f>
-        <v>1.3417906318580169E-21</v>
+        <f>$C12*F3*F5</f>
+        <v>4.3057350240366027E-10</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>10</v>
       </c>
-      <c r="B13" s="20" t="str">
+      <c r="B13" t="str">
         <v>DonnanFA-Cu</v>
       </c>
-      <c r="C13" s="20">
-        <f ca="1"/>
+      <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" s="18">
-        <f ca="1">$C13*D3*D7^2</f>
-        <v>9.9999887798122902E-7</v>
+        <f>IF(D32&lt;0,$C13*D3*D7^2,0)</f>
+        <v>507365.15176796808</v>
       </c>
       <c r="E13" s="18">
-        <f ca="1">$C13*E3*E7^2</f>
-        <v>1.0866808053901159E-6</v>
+        <f>IF(E32&lt;0,$C13*E3*E7^2,0)</f>
+        <v>507365.15176796808</v>
       </c>
       <c r="F13" s="18">
-        <f ca="1">$C13*F3*F7^2</f>
-        <v>1.9999977559624581E-18</v>
+        <f>IF(F32&lt;0,$C13*F3*F7^2,0)</f>
+        <v>507365.15176796808</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="21">
+      <c r="A14">
         <v>11</v>
       </c>
-      <c r="B14" s="20" t="str">
+      <c r="B14" t="str">
         <v>DonnanFA-Na</v>
       </c>
-      <c r="C14" s="20">
-        <f ca="1"/>
+      <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" s="18">
-        <f ca="1">$C14*D4*D7</f>
-        <v>9.9999900000099996E-4</v>
+        <f>IF(D32&lt;0,$C14*D4*D7,0)</f>
+        <v>889.12737023894613</v>
       </c>
       <c r="E14" s="18">
-        <f ca="1">$C14*E4*E7</f>
-        <v>1E-3</v>
+        <f>IF(E32&lt;0,$C14*E4*E7,0)</f>
+        <v>889.12737023894613</v>
       </c>
       <c r="F14" s="18">
-        <f ca="1">$C14*F4*F7</f>
-        <v>5.0000000000000001E-4</v>
+        <f>IF(F32&lt;0,$C14*F4*F7,0)</f>
+        <v>889.12737023894613</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="21">
+      <c r="A15">
         <v>12</v>
       </c>
-      <c r="B15" s="20" t="str">
+      <c r="B15" s="28" t="str">
         <v>DonnanFA-Cl</v>
       </c>
-      <c r="C15" s="20">
-        <f ca="1"/>
+      <c r="C15" s="28">
         <v>1</v>
       </c>
       <c r="D15" s="18">
-        <f ca="1">$C$15*D5*D7</f>
-        <v>2.99999700000299E-4</v>
+        <f>IF(D32&lt;0,0,$C$15*D5*D7)</f>
+        <v>0</v>
       </c>
       <c r="E15" s="18">
-        <f ca="1">$C$15*E5*E7</f>
-        <v>5.9999999938594513E-4</v>
+        <f>IF(E32&lt;0,0,$C$15*E5*E7)</f>
+        <v>0</v>
       </c>
       <c r="F15" s="18">
-        <f ca="1">$C$15*F5*F7</f>
-        <v>2.9999999969297257E-4</v>
+        <f>IF(F32&lt;0,0,$C$15*F5*F7)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>13</v>
       </c>
-      <c r="B16" s="20" t="str">
+      <c r="B16" t="str">
         <v>DonnanFA-H</v>
       </c>
-      <c r="C16" s="20">
-        <f ca="1"/>
+      <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" s="18">
-        <f ca="1">$C$16*D6*D7</f>
-        <v>2.6915348039269101E-2</v>
+        <f>IF(D32&lt;0,$C$16*D6*D7,0)</f>
+        <v>2.393117262122155E-2</v>
       </c>
       <c r="E16" s="18">
-        <f ca="1">$C$16*E6*E7</f>
-        <v>5.3830696078538202E-8</v>
+        <f>IF(E32&lt;0,$C$16*E6*E7,0)</f>
+        <v>2.393117262122155E-2</v>
       </c>
       <c r="F16" s="18">
-        <f ca="1">$C$16*F6*F7</f>
-        <v>2.6915348039269101E-8</v>
+        <f>IF(F32&lt;0,$C$16*F6*F7,0)</f>
+        <v>2.393117262122155E-2</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
+      <c r="A17">
         <v>14</v>
       </c>
-      <c r="B17" s="20" t="str">
+      <c r="B17" s="28" t="str">
         <v>DonnanFA-OH</v>
       </c>
-      <c r="C17" s="20">
-        <f ca="1"/>
+      <c r="C17" s="28">
         <v>1.0069316688518E-14</v>
       </c>
       <c r="D17" s="18">
-        <f ca="1">$C$17*D7/D6</f>
-        <v>0.37411058827205257</v>
+        <f>IF(D32&lt;0,0,$C$17*D7/D6)</f>
+        <v>0</v>
       </c>
       <c r="E17" s="18">
-        <f ca="1">$C$17*E7/E6</f>
-        <v>7.482211765441051E-7</v>
+        <f>IF(E32&lt;0,0,$C$17*E7/E6)</f>
+        <v>0</v>
       </c>
       <c r="F17" s="18">
-        <f ca="1">$C$17*F7/F6</f>
-        <v>3.7411058827205255E-7</v>
+        <f>IF(F32&lt;0,0,$C$17*F7/F6)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="21">
+      <c r="A18">
         <v>15</v>
       </c>
-      <c r="B18" s="20" t="str">
+      <c r="B18" t="str">
         <v>DonnanFA-CuOH</v>
       </c>
-      <c r="C18" s="20">
-        <f ca="1"/>
+      <c r="C18">
         <v>3.0199517204020201E-8</v>
       </c>
       <c r="D18" s="18">
-        <f ca="1">$C$18*D3/D6*D7</f>
-        <v>1.1220171953762002E-12</v>
+        <f>IF(D32&lt;0,$C$18*D3/D6*D7,0)</f>
+        <v>0.64026041983207105</v>
       </c>
       <c r="E18" s="18">
-        <f ca="1">$C$18*E3/E6*E7</f>
-        <v>6.0963795879171736E-7</v>
+        <f>IF(E32&lt;0,$C$18*E3/E6*E7,0)</f>
+        <v>0.64026041983207105</v>
       </c>
       <c r="F18" s="18">
-        <f ca="1">$C$18*F3/F6*F7</f>
-        <v>2.2440343907524003E-18</v>
+        <f>IF(F32&lt;0,$C$18*F3/F6*F7,0)</f>
+        <v>0.64026041983207105</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>16</v>
       </c>
-      <c r="B19" s="20" t="str">
+      <c r="B19" t="str">
         <v>DonnanFA-CuCl</v>
       </c>
-      <c r="C19" s="20">
-        <f ca="1"/>
+      <c r="C19">
         <v>2.5118864315095801</v>
       </c>
       <c r="D19" s="18">
-        <f ca="1">$C$19*D3*D5</f>
-        <v>7.5356433037342313E-28</v>
+        <f>IF(D32&lt;0,$C$19*D3*D5,0)</f>
+        <v>4.8363008273328873E-10</v>
       </c>
       <c r="E19" s="18">
-        <f ca="1">$C$19*E3*E5</f>
-        <v>2.0472140757358315E-10</v>
+        <f>IF(E32&lt;0,$C$19*E3*E5,0)</f>
+        <v>4.8363008273328873E-10</v>
       </c>
       <c r="F19" s="18">
-        <f ca="1">$C$19*F3*F5</f>
-        <v>1.5071301663330779E-21</v>
+        <f>IF(F32&lt;0,$C$19*F3*F5,0)</f>
+        <v>4.8363008273328873E-10</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="21">
+      <c r="A20">
         <v>17</v>
       </c>
-      <c r="B20" s="20" t="str">
+      <c r="B20" t="str">
         <v>DOC-FA_1</v>
       </c>
-      <c r="C20" s="20">
-        <f ca="1"/>
-        <v>2.5703957827688601E-2</v>
+      <c r="C20">
+        <v>2.5702734809241599E-2</v>
       </c>
       <c r="D20" s="18">
-        <f ca="1">$C$20*D8/D6</f>
-        <v>7.0949925706307208E-7</v>
+        <f>$C$20*D8/D6</f>
+        <v>7.0945954064074083E-8</v>
       </c>
       <c r="E20" s="18">
-        <f ca="1">$C$20*E8/E6</f>
-        <v>7.0949925506216604E-8</v>
+        <f>$C$20*E8/E6</f>
+        <v>7.0945954064074083E-8</v>
       </c>
       <c r="F20" s="18">
-        <f ca="1">$C$20*F8/F6</f>
-        <v>7.0949925506216604E-8</v>
+        <f>$C$20*F8/F6</f>
+        <v>7.0945954064074083E-8</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="21">
+      <c r="A21">
         <v>18</v>
       </c>
-      <c r="B21" s="20" t="str">
+      <c r="B21" t="str">
         <v>DOC-FA_8</v>
       </c>
-      <c r="C21" s="20">
-        <f ca="1"/>
-        <v>3.9810717055349702E-13</v>
+      <c r="C21" s="18">
+        <v>3.98088228240536E-13</v>
       </c>
       <c r="D21" s="18">
-        <f ca="1">$C$21*D9/D6</f>
-        <v>5.2470593973307545E-12</v>
+        <f>$C$21*D9/D6</f>
+        <v>5.0724800624993542E-13</v>
       </c>
       <c r="E21" s="18">
-        <f ca="1">$C$21*E9/E6</f>
-        <v>5.2469988381521492E-13</v>
+        <f>$C$21*E9/E6</f>
+        <v>5.0724800624993542E-13</v>
       </c>
       <c r="F21" s="18">
-        <f ca="1">$C$21*F9/F6</f>
-        <v>5.2469988381521492E-13</v>
+        <f>$C$21*F9/F6</f>
+        <v>5.0724800624993542E-13</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>19</v>
       </c>
-      <c r="B22" s="20" t="str">
+      <c r="B22" t="str">
         <v>DOC-FA_1-Cu</v>
       </c>
-      <c r="C22" s="20">
-        <f ca="1"/>
-        <v>0.15848931924611101</v>
+      <c r="C22">
+        <v>0.158481778175495</v>
       </c>
       <c r="D22" s="18">
-        <f ca="1">$C$22*D3/D6*D8</f>
-        <v>4.3747320487582642E-24</v>
+        <f>$C$22*D3/D6*D8</f>
+        <v>2.807503517019703E-13</v>
       </c>
       <c r="E22" s="18">
-        <f ca="1">$C$22*E3/E6*E8</f>
-        <v>1.1884856666791491E-13</v>
+        <f>$C$22*E3/E6*E8</f>
+        <v>2.807503517019703E-13</v>
       </c>
       <c r="F22" s="18">
-        <f ca="1">$C$22*F3/F6*F8</f>
-        <v>8.7494640728415846E-25</v>
+        <f>$C$22*F3/F6*F8</f>
+        <v>2.807503517019703E-13</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="21">
+      <c r="A23">
         <v>20</v>
       </c>
-      <c r="B23" s="20" t="str">
+      <c r="B23" t="str">
         <v>DOC-FA_8-Cu</v>
       </c>
-      <c r="C23" s="20">
-        <f ca="1"/>
-        <v>6.7920363261718397E-4</v>
+      <c r="C23">
+        <v>6.7917131547063595E-4</v>
       </c>
       <c r="D23" s="18">
-        <f ca="1">$C$23*D3/D6*D9</f>
-        <v>8.9519055876219664E-21</v>
+        <f>$C$23*D3/D6*D9</f>
+        <v>5.5540914249206579E-10</v>
       </c>
       <c r="E23" s="18">
-        <f ca="1">$C$23*E3/E6*E9</f>
-        <v>2.4319406534684487E-10</v>
+        <f>$C$23*E3/E6*E9</f>
+        <v>5.5540914249206579E-10</v>
       </c>
       <c r="F23" s="18">
-        <f ca="1">$C$23*F3/F6*F9</f>
-        <v>1.7903604537579557E-21</v>
+        <f>$C$23*F3/F6*F9</f>
+        <v>5.5540914249206579E-10</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="21">
+      <c r="A24">
         <v>21</v>
       </c>
-      <c r="B24" s="20" t="str">
+      <c r="B24" t="str">
         <v>DOC-FA_1-CuOH</v>
       </c>
-      <c r="C24" s="20">
-        <f ca="1"/>
+      <c r="C24" s="18">
         <v>4.7863009232263802E-9</v>
       </c>
       <c r="D24" s="18">
-        <f ca="1">$C$24*D3/D6^2*D7</f>
-        <v>6.6069270669714773E-6</v>
+        <f>$C$24*D3/D6^2*D7</f>
+        <v>3770132.8599342071</v>
       </c>
       <c r="E24" s="18">
-        <f ca="1">$C$24*E3/E6^2*E7</f>
-        <v>3.5898144409843478</v>
+        <f>$C$24*E3/E6^2*E7</f>
+        <v>3770132.8599342071</v>
       </c>
       <c r="F24" s="18">
-        <f ca="1">$C$24*F3/F6^2*F7</f>
-        <v>1.3213854133942955E-11</v>
+        <f>$C$24*F3/F6^2*F7</f>
+        <v>3770132.8599342071</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>22</v>
       </c>
-      <c r="B25" s="20" t="str">
+      <c r="B25" t="str">
         <v>DOC-FA_8-CuOH</v>
       </c>
-      <c r="C25" s="20">
-        <f ca="1"/>
+      <c r="C25" s="18">
         <v>2.0511621788255701E-11</v>
       </c>
       <c r="D25" s="18">
-        <f ca="1">$C$25*D3/D6^2*D8</f>
-        <v>2.1035433079670832E-26</v>
+        <f>$C$25*D3/D6^2*D8</f>
+        <v>1.3500223972272858E-15</v>
       </c>
       <c r="E25" s="18">
-        <f ca="1">$C$25*E3/E6^2*E8</f>
-        <v>5.7147067360784694E-16</v>
+        <f>$C$25*E3/E6^2*E8</f>
+        <v>1.3500223972272858E-15</v>
       </c>
       <c r="F25" s="18">
-        <f ca="1">$C$25*F3/F6^2*F8</f>
-        <v>4.2070866040694828E-27</v>
-      </c>
+        <f>$C$25*F3/F6^2*F8</f>
+        <v>1.3500223972272858E-15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="20" t="s">
+      <c r="B27" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" s="18">
+        <v>8.0000000000000003E-10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="18">
+        <v>1.06425E-7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C30" s="18"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C31" s="18"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" s="18">
+        <f>(D20*-1+D21*-1+D22*1+D23*1)*C35</f>
+        <v>-7.0390771419236563E-8</v>
+      </c>
+      <c r="E32" s="18">
+        <f>(E20*-1+E21*-1+E22*1+E23*1)*D35</f>
+        <v>-7.0390768690696464E-8</v>
+      </c>
+      <c r="F32" s="18">
+        <f>(F20*-1+F21*-1+F22*1+F23*1)*E35</f>
+        <v>-7.0390771402628973E-8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="18">
+        <f>((D3*4+D4*1+D5*1+D6*1+D10*1+D11*1+D12*1+D20*1+D21*1+D22*1+D23*1)*C35+(D13*4+D14*1+D15*1+D16*1+D17*1+D18*1+D19*1)*C36)*0.5</f>
+        <v>6.5191969040583465E-4</v>
+      </c>
+      <c r="E33" s="18">
+        <f>((E3*4+E4*1+E5*1+E6*1+E10*1+E11*1+E12*1+E20*1+E21*1+E22*1+E23*1)*D35+(E13*4+E14*1+E15*1+E16*1+E17*1+E18*1+E19*1)*D36)*0.5</f>
+        <v>4.000290536479708E-2</v>
+      </c>
+      <c r="F33" s="18">
+        <f>((F3*4+F4*1+F5*1+F6*1+F10*1+F11*1+F12*1+F20*1+F21*1+F22*1+F23*1)*E35+(F13*4+F14*1+F15*1+F16*1+F17*1+F18*1+F19*1)*E36)*0.5</f>
+        <v>8.914343567261628E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="18">
+        <f>(1000*(6.022E+23)/$C$27*4*PI()/3*($C$28+(0.000000000304/SQRT(D33)))^3-($C$28^3))*1000*ABS(D32)/(1+1000*ABS(D32))*$C$29*$C$27</f>
+        <v>3.8762759204089525E-8</v>
+      </c>
+      <c r="E34" s="18">
+        <f>(1000*(6.022E+23)/$C$27*4*PI()/3*($C$28+(0.000000000304/SQRT(E33)))^3-($C$28^3))*1000*ABS(E32)/(1+1000*ABS(E32))*$C$29*$C$27</f>
+        <v>2.3593431643277636E-10</v>
+      </c>
+      <c r="F34" s="18">
+        <f>(1000*(6.022E+23)/$C$27*4*PI()/3*($C$28+(0.000000000304/SQRT(F33)))^3-($C$28^3))*1000*ABS(F32)/(1+1000*ABS(F32))*$C$29*$C$27</f>
+        <v>2.5025964813669127E-8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" s="18">
+        <f>1-C36</f>
+        <v>1</v>
+      </c>
+      <c r="D35" s="18">
+        <f>1-D36</f>
+        <v>0.99999996123724677</v>
+      </c>
+      <c r="E35" s="18">
+        <f>1-E36</f>
+        <v>0.99999999976406573</v>
+      </c>
+      <c r="F35" s="18">
+        <f>1-F36</f>
+        <v>0.9999999749740377</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="18">
+        <v>9.9999999999999904E-21</v>
+      </c>
+      <c r="D36" s="18">
+        <f>0.25 / (0.25+D34)*D34</f>
+        <v>3.876275319388445E-8</v>
+      </c>
+      <c r="E36" s="18">
+        <f>0.25 / (0.25+E34)*E34</f>
+        <v>2.3593431621011635E-10</v>
+      </c>
+      <c r="F36" s="18">
+        <f>0.25 / (0.25+F34)*F34</f>
+        <v>2.5025962308473719E-8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" s="18">
+        <f>(2*D13+D14+D15+D16+D17+D18+D19)*C36</f>
+        <v>1.0156200950977672E-14</v>
+      </c>
+      <c r="E37" s="18">
+        <f>(2*E13+E14+E15+E16+E17+E18+E19)*D36</f>
+        <v>3.9368231085024241E-2</v>
+      </c>
+      <c r="F37" s="18">
+        <f>(2*F13+F14+F15+F16+F17+F18+F19)*E36</f>
+        <v>2.3961963266614527E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>115</v>
+      </c>
+      <c r="D38" s="18">
+        <f>D37-ABS(D32)</f>
+        <v>-7.0390761263035618E-8</v>
+      </c>
+      <c r="E38" s="18">
+        <f>E37-ABS(E32)</f>
+        <v>3.9368160694255548E-2</v>
+      </c>
+      <c r="F38" s="18">
+        <f>F37-ABS(F32)</f>
+        <v>2.3954924189474263E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B40" t="s">
+        <v>105</v>
+      </c>
+      <c r="D40" s="18">
+        <f>(2*D7*D3*$C$13+D3*D6^-1*$C$18+D3*D5*$C$19)</f>
+        <v>1.1412661202338799</v>
+      </c>
+      <c r="E40" s="18">
+        <f>E36*(2*E7*E3*$C$13+E3*E6^-1*$C$18+E3*E5*$C$19)</f>
+        <v>2.6926384169115288E-10</v>
+      </c>
+      <c r="F40" s="18">
+        <f>F36*(2*F7*F3*$C$13+F3*F6^-1*$C$18+F3*F5*$C$19)</f>
+        <v>2.8561282908911113E-8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" t="s">
+        <v>106</v>
+      </c>
+      <c r="D41" s="18">
+        <f>D4*$C$14</f>
+        <v>9.9999999999999005E-4</v>
+      </c>
+      <c r="E41" s="18">
+        <f>E4*$C$14*E36</f>
+        <v>2.3593431621011401E-13</v>
+      </c>
+      <c r="F41" s="18">
+        <f>F4*$C$14*F36</f>
+        <v>2.5025962308473469E-11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" t="s">
+        <v>107</v>
+      </c>
+      <c r="D42" s="18">
+        <f>D3*D5*$C$19</f>
+        <v>4.8363008273328863E-10</v>
+      </c>
+      <c r="E42" s="18">
+        <f>E3*E5*$C$19*E36</f>
+        <v>1.1410493286832044E-19</v>
+      </c>
+      <c r="F42" s="18">
+        <f>F3*F5*$C$19*F36</f>
+        <v>1.2103308221727307E-17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B43" t="s">
         <v>101</v>
       </c>
-      <c r="D27" s="18">
-        <v>-7.0960162187784801E-7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="20" t="s">
+      <c r="D43" s="18">
+        <f>(2*D7^2*$C$13+D7*D6^-1*$C$18+D7*D5*$C$19)</f>
+        <v>1581095959303.4124</v>
+      </c>
+      <c r="E43" s="18">
+        <f>E36*(2*E7^2*$C$13+E7*E6^-1*$C$18+E7*E5*$C$19)</f>
+        <v>373.03479402082854</v>
+      </c>
+      <c r="F43" s="18">
+        <f>F36*(2*F7^2*$C$13+F7*F6^-1*$C$18+F7*F5*$C$19)</f>
+        <v>39568.447883607296</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B44" t="s">
         <v>102</v>
       </c>
-      <c r="D28" s="18">
-        <v>1.4427199424933401E-10</v>
+      <c r="D44" s="18">
+        <f>D7*$C$14</f>
+        <v>889127.37023895502</v>
+      </c>
+      <c r="E44" s="18">
+        <f>E7*$C$14*E36</f>
+        <v>2.0977565812102679E-4</v>
+      </c>
+      <c r="F44" s="18">
+        <f>F7*$C$14*F36</f>
+        <v>2.2251268055032445E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B45" t="s">
+        <v>103</v>
+      </c>
+      <c r="D45" s="18">
+        <f>(D7*D3*$C$19)</f>
+        <v>1.4333645360666922</v>
+      </c>
+      <c r="E45" s="18">
+        <f>E36*(E7*E3*$C$19)</f>
+        <v>3.3817988169672569E-10</v>
+      </c>
+      <c r="F45" s="18">
+        <f>F36*(F7*F3*$C$19)</f>
+        <v>3.5871326853907958E-8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B46" t="s">
+        <v>104</v>
+      </c>
+      <c r="D46" s="18">
+        <f>(4*D7*D3*$C$13+D4*$C$14+D6*$C$16+D3*D6^-1*$C$18+D3*D5*$C$19)</f>
+        <v>2.2835315467997024</v>
+      </c>
+      <c r="E46" s="18">
+        <f>E36*(4*E7*E3*$C$13+E4*$C$14+E6*$C$16+E3*E6^-1*$C$18+E3*E5*$C$19)</f>
+        <v>5.3876345403841711E-10</v>
+      </c>
+      <c r="F46" s="18">
+        <f>F36*(4*F7*F3*$C$13+F4*$C$14+F6*$C$16+F3*F6^-1*$C$18+F3*F5*$C$19)</f>
+        <v>5.7147574420420045E-8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D48" s="18">
+        <f>((2*D13+D18+D19)*D36)/(D3*D35)</f>
+        <v>61287.634796031998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>